<commit_message>
Cleaned up level folder
Also fixed a bug with disabled screenshake and updated localization
files.
</commit_message>
<xml_diff>
--- a/godot_project/strings.xlsx
+++ b/godot_project/strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GameDev\star_breaker\godot_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GameDev\danger-chasers\godot_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FBF972C4-04CA-406D-B2ED-C4711E24938E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F0615FE-B029-449B-A8AD-FA424BC7AFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19275" yWindow="4260" windowWidth="15300" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3240" windowWidth="21600" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strings" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>NONE</t>
   </si>
   <si>
-    <t>Streams of Steel</t>
-  </si>
-  <si>
     <t>New Game</t>
   </si>
   <si>
@@ -232,40 +229,151 @@
     <t>Quests</t>
   </si>
   <si>
-    <t>TRIAL_RUN</t>
-  </si>
-  <si>
-    <t>TRIAL_RUN_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>FOREST_GROVE</t>
-  </si>
-  <si>
-    <t>FOREST_GROVE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>SAFE_AREA_CR-1</t>
-  </si>
-  <si>
-    <t>SAFE_AREA_CR-1_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Trial Run</t>
-  </si>
-  <si>
-    <t>Forest Grove</t>
-  </si>
-  <si>
-    <t>A safe area inside the Greenwood Hills. Travelers frequently use this place to rest on their trip to the Ruby Mines. A fellow adventurer seems to want to spar here though...</t>
-  </si>
-  <si>
-    <t>Safe Area CR-1</t>
-  </si>
-  <si>
-    <t>CR is the code used to denote rest areas in the Ruby Mines. You've been ambushed by a peculiar maid, but it doesn't look like she wants to injure you. At least that's what you think.</t>
-  </si>
-  <si>
-    <t>The forest right outside this city is filled with dangerous creatures to the average citizen. However, since they are pretty weak overall, we leave them be. We send new adventurers after them to test their capabilities and decide what to do based on that performance. Well, good luck!</t>
+    <t>EXIT</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>AUDIO</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>GRAPHICS</t>
+  </si>
+  <si>
+    <t>Graphics</t>
+  </si>
+  <si>
+    <t>SCREEN_SHAKE</t>
+  </si>
+  <si>
+    <t>Screen Shake</t>
+  </si>
+  <si>
+    <t>FRAME_FREEZE</t>
+  </si>
+  <si>
+    <t>Frame Freeze</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>On</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>DISABLED</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>NORMAL</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>EXTREME</t>
+  </si>
+  <si>
+    <t>VOMIT</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Extreme</t>
+  </si>
+  <si>
+    <t>Vomit</t>
+  </si>
+  <si>
+    <t>ZERO_LIMIT</t>
+  </si>
+  <si>
+    <t>Zero Limit</t>
+  </si>
+  <si>
+    <t>ACT</t>
+  </si>
+  <si>
+    <t>Act</t>
+  </si>
+  <si>
+    <t>Zero Limit Act 1</t>
+  </si>
+  <si>
+    <t>ZERO_LIMIT_ACT_2</t>
+  </si>
+  <si>
+    <t>ZERO_LIMIT_ACT_1</t>
+  </si>
+  <si>
+    <t>insert description here lol</t>
+  </si>
+  <si>
+    <t>Zero Limit Act 2</t>
+  </si>
+  <si>
+    <t>ZERO_LIMIT_ACT_2_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>this is where I explain the story for now but nothing is here because reeeeeeeeee</t>
+  </si>
+  <si>
+    <t>DEBUG_ENEMY</t>
+  </si>
+  <si>
+    <t>Debug Enemy</t>
+  </si>
+  <si>
+    <t>DEBUG_ENEMY_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>I put enemies in here and test them out to make sure that they try to kill you the correct way.</t>
+  </si>
+  <si>
+    <t>DECLINE</t>
+  </si>
+  <si>
+    <t>Decline</t>
+  </si>
+  <si>
+    <t>ACCEPT</t>
+  </si>
+  <si>
+    <t>Accept</t>
+  </si>
+  <si>
+    <t>ZERO_LIMIT_ACT_1_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Danger Chaser</t>
   </si>
 </sst>
 </file>
@@ -1106,97 +1214,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1204,247 +1307,391 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
         <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
         <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
         <v>35</v>
-      </c>
-      <c r="B34" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>65</v>
+      </c>
+      <c r="B100" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>67</v>
+      </c>
+      <c r="B101" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>99</v>
+      </c>
+      <c r="B102" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>97</v>
+      </c>
+      <c r="B103" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>116</v>
+      </c>
+      <c r="B105" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>102</v>
+      </c>
+      <c r="B106" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>110</v>
+      </c>
+      <c r="B109" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added option to switch between windowed and full screen
</commit_message>
<xml_diff>
--- a/godot_project/strings.xlsx
+++ b/godot_project/strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GameDev\danger-chasers\godot_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F424795-55DE-401C-B2BB-47C990EAF502}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4384DF15-BF38-4542-B8A3-07BFA60BE456}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="3240" windowWidth="21600" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>NONE</t>
   </si>
@@ -374,6 +374,24 @@
   </si>
   <si>
     <t>this is where I explain the story for now but nothing is here because oops</t>
+  </si>
+  <si>
+    <t>WINDOW_MODE</t>
+  </si>
+  <si>
+    <t>Window Mode</t>
+  </si>
+  <si>
+    <t>WINDOWED</t>
+  </si>
+  <si>
+    <t>Windowed</t>
+  </si>
+  <si>
+    <t>FULL_SCREEN</t>
+  </si>
+  <si>
+    <t>Full Screen</t>
   </si>
 </sst>
 </file>
@@ -1216,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,6 +1632,30 @@
         <v>114</v>
       </c>
     </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" t="s">
+        <v>123</v>
+      </c>
+    </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Official public build 0.6.1
Features: 2 levels: Zero Limit Acts 1 and 2.

Barebones tutorial, no story or cutscenes or whatever, low framerate in
areas with that cave background (that's most likely an issue with
ParallaxLayers combined with Tilemaps in Godot. I believe I could
probably fix that if I just converted those background tilemaps into
sprites instead. Off topic)

Also released to the public on itch.io! Conffetti wheeeeeeeeeee
</commit_message>
<xml_diff>
--- a/godot_project/strings.xlsx
+++ b/godot_project/strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GameDev\danger-chasers\godot_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4384DF15-BF38-4542-B8A3-07BFA60BE456}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A34672-DB33-4EF0-9088-8148BE8A5C6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="3240" windowWidth="21600" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>NONE</t>
   </si>
@@ -373,9 +373,6 @@
     <t>Danger Chaser</t>
   </si>
   <si>
-    <t>this is where I explain the story for now but nothing is here because oops</t>
-  </si>
-  <si>
     <t>WINDOW_MODE</t>
   </si>
   <si>
@@ -392,6 +389,21 @@
   </si>
   <si>
     <t>Full Screen</t>
+  </si>
+  <si>
+    <t>ZERO_LIMIT_ACT_3</t>
+  </si>
+  <si>
+    <t>ZERO_LIMIT_ACT_3_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Zero Limit Act 3</t>
+  </si>
+  <si>
+    <t>This is supposed to be an easy tutorial stage for the player to get used to the controls.</t>
+  </si>
+  <si>
+    <t>Another easy tutorial stage. This one has some "Arenas" that you can't pass until you beat all the enemies. More combat focused than the first level, but you can also skip a lot of encounters.</t>
   </si>
 </sst>
 </file>
@@ -1232,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B109"/>
+  <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,26 +1646,26 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" t="s">
         <v>118</v>
-      </c>
-      <c r="B51" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" t="s">
         <v>120</v>
-      </c>
-      <c r="B52" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>121</v>
+      </c>
+      <c r="B53" t="s">
         <v>122</v>
-      </c>
-      <c r="B53" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1701,7 +1713,7 @@
         <v>115</v>
       </c>
       <c r="B105" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -1717,22 +1729,38 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="B108" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>124</v>
+      </c>
+      <c r="B109" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>107</v>
+      </c>
+      <c r="B110" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>109</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B111" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated main menu, pause menu
Also updated localization files.
</commit_message>
<xml_diff>
--- a/godot_project/strings.xlsx
+++ b/godot_project/strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GameDev\danger-chasers\godot_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A34672-DB33-4EF0-9088-8148BE8A5C6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EDC0AA-EF45-4A85-9B5F-7D01F9A30CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3240" windowWidth="21600" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3345" yWindow="2565" windowWidth="23790" windowHeight="12465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strings" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="132">
   <si>
     <t>NONE</t>
   </si>
@@ -370,9 +370,6 @@
     <t>ZERO_LIMIT_ACT_1_DESCRIPTION</t>
   </si>
   <si>
-    <t>Danger Chaser</t>
-  </si>
-  <si>
     <t>WINDOW_MODE</t>
   </si>
   <si>
@@ -404,6 +401,21 @@
   </si>
   <si>
     <t>Another easy tutorial stage. This one has some "Arenas" that you can't pass until you beat all the enemies. More combat focused than the first level, but you can also skip a lot of encounters.</t>
+  </si>
+  <si>
+    <t>EXIT TO DESKTOP</t>
+  </si>
+  <si>
+    <t>Exit to Desktop</t>
+  </si>
+  <si>
+    <t>Danger Chasers</t>
+  </si>
+  <si>
+    <t>PRESS ANY BUTTON</t>
+  </si>
+  <si>
+    <t>Press Any Button</t>
   </si>
 </sst>
 </file>
@@ -1244,10 +1256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B111"/>
+  <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,7 +1277,7 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1646,26 +1658,26 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51" t="s">
         <v>117</v>
-      </c>
-      <c r="B51" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" t="s">
         <v>119</v>
-      </c>
-      <c r="B52" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>120</v>
+      </c>
+      <c r="B53" t="s">
         <v>121</v>
-      </c>
-      <c r="B53" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1713,7 +1725,7 @@
         <v>115</v>
       </c>
       <c r="B105" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -1729,20 +1741,20 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B108" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B109" t="s">
         <v>104</v>
@@ -1762,6 +1774,30 @@
       </c>
       <c r="B111" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>127</v>
+      </c>
+      <c r="B112" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>61</v>
+      </c>
+      <c r="B113" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>130</v>
+      </c>
+      <c r="B114" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added base for InnerSpectre
</commit_message>
<xml_diff>
--- a/godot_project/strings.xlsx
+++ b/godot_project/strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GameDev\danger-chasers\godot_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EDC0AA-EF45-4A85-9B5F-7D01F9A30CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD04DC2B-D341-412C-85F5-264C9AD2408A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="2565" windowWidth="23790" windowHeight="12465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strings" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="135">
   <si>
     <t>NONE</t>
   </si>
@@ -416,6 +416,15 @@
   </si>
   <si>
     <t>Press Any Button</t>
+  </si>
+  <si>
+    <t>Don't you want something more?</t>
+  </si>
+  <si>
+    <t>Make up for lost time?</t>
+  </si>
+  <si>
+    <t>Then prove it to me.</t>
   </si>
 </sst>
 </file>
@@ -1256,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B114"/>
+  <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,6 +1809,30 @@
         <v>131</v>
       </c>
     </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>132</v>
+      </c>
+      <c r="B126" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>133</v>
+      </c>
+      <c r="B127" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>134</v>
+      </c>
+      <c r="B128" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>